<commit_message>
Update PVenta.xlsx structure / Updating Service Rol and controller to MessageApp
</commit_message>
<xml_diff>
--- a/PVenta.BD/PVenta.xlsx
+++ b/PVenta.BD/PVenta.xlsx
@@ -5,30 +5,32 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DesaVisual\PVenta\PVenta BD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DesaVisual\PVenta\PVenta.BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraSist" sheetId="1" r:id="rId1"/>
-    <sheet name="1. LogEventos" sheetId="4" r:id="rId2"/>
-    <sheet name="15. ErrorList" sheetId="17" r:id="rId3"/>
-    <sheet name="2. Roles" sheetId="2" r:id="rId4"/>
-    <sheet name="3. Usuarios" sheetId="3" r:id="rId5"/>
-    <sheet name="4. OpcionesSist" sheetId="5" r:id="rId6"/>
-    <sheet name="5. PermisosRoles" sheetId="6" r:id="rId7"/>
-    <sheet name="6. Mesas" sheetId="7" r:id="rId8"/>
-    <sheet name="7. Monedas" sheetId="8" r:id="rId9"/>
-    <sheet name="8. Categorias" sheetId="9" r:id="rId10"/>
-    <sheet name="9. Productos" sheetId="10" r:id="rId11"/>
-    <sheet name="10. FacturaHeader" sheetId="11" r:id="rId12"/>
-    <sheet name="11. FacturaDetail" sheetId="12" r:id="rId13"/>
-    <sheet name="12. FacturaPayment" sheetId="15" r:id="rId14"/>
-    <sheet name="13. CuadreHeader" sheetId="13" r:id="rId15"/>
-    <sheet name="14. CuadreDetail" sheetId="14" r:id="rId16"/>
-    <sheet name="Seguridad" sheetId="16" r:id="rId17"/>
+    <sheet name="1. ErrorList" sheetId="17" r:id="rId2"/>
+    <sheet name="2. Roles" sheetId="2" r:id="rId3"/>
+    <sheet name="3. Usuarios" sheetId="3" r:id="rId4"/>
+    <sheet name="4. LogEventos" sheetId="4" r:id="rId5"/>
+    <sheet name="5. OpcionesSist" sheetId="5" r:id="rId6"/>
+    <sheet name="6. PermisosRoles" sheetId="6" r:id="rId7"/>
+    <sheet name="7. Mesas" sheetId="7" r:id="rId8"/>
+    <sheet name="8. Monedas" sheetId="8" r:id="rId9"/>
+    <sheet name="9. Categorias" sheetId="9" r:id="rId10"/>
+    <sheet name="10. Productos" sheetId="10" r:id="rId11"/>
+    <sheet name="11. OrderHeader " sheetId="18" r:id="rId12"/>
+    <sheet name="12. OrderDetail " sheetId="19" r:id="rId13"/>
+    <sheet name="13. FacturaHeader" sheetId="11" r:id="rId14"/>
+    <sheet name="14. FacturaDetail" sheetId="12" r:id="rId15"/>
+    <sheet name="15. FacturaPayment" sheetId="15" r:id="rId16"/>
+    <sheet name="16. CuadreHeader" sheetId="13" r:id="rId17"/>
+    <sheet name="17. CuadreDetail" sheetId="14" r:id="rId18"/>
+    <sheet name="Seguridad" sheetId="16" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="101">
   <si>
     <t>Roles</t>
   </si>
@@ -337,6 +339,12 @@
   </si>
   <si>
     <t>Registro Actualizado</t>
+  </si>
+  <si>
+    <t>OrderHID</t>
+  </si>
+  <si>
+    <t>ErrorListId</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1258,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,7 +1440,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>49</v>
@@ -1509,6 +1517,280 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -1607,7 +1889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -1730,7 +2012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -1738,7 +2020,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,7 +2095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D9"/>
   <sheetViews>
@@ -1953,103 +2235,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FF92D050"/>
-  </sheetPr>
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2181,7 +2372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -2253,7 +2444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -2368,6 +2559,97 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding FormaPago Models, Service and Controller
</commit_message>
<xml_diff>
--- a/PVenta.BD/PVenta.xlsx
+++ b/PVenta.BD/PVenta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" firstSheet="15" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraSist" sheetId="1" r:id="rId1"/>
@@ -21,16 +21,17 @@
     <sheet name="6. PermisosRoles" sheetId="6" r:id="rId7"/>
     <sheet name="7. Mesas" sheetId="7" r:id="rId8"/>
     <sheet name="8. Monedas" sheetId="8" r:id="rId9"/>
-    <sheet name="9. Categorias" sheetId="9" r:id="rId10"/>
-    <sheet name="10. Productos" sheetId="10" r:id="rId11"/>
-    <sheet name="11. OrderHeader " sheetId="18" r:id="rId12"/>
-    <sheet name="12. OrderDetail " sheetId="19" r:id="rId13"/>
-    <sheet name="13. FacturaHeader" sheetId="11" r:id="rId14"/>
-    <sheet name="14. FacturaDetail" sheetId="12" r:id="rId15"/>
-    <sheet name="15. FacturaPayment" sheetId="15" r:id="rId16"/>
-    <sheet name="16. CuadreHeader" sheetId="13" r:id="rId17"/>
-    <sheet name="17. CuadreDetail" sheetId="14" r:id="rId18"/>
-    <sheet name="Seguridad" sheetId="16" r:id="rId19"/>
+    <sheet name="9 FormaPago" sheetId="20" r:id="rId10"/>
+    <sheet name="9. Categorias" sheetId="9" r:id="rId11"/>
+    <sheet name="10. Productos" sheetId="10" r:id="rId12"/>
+    <sheet name="11. OrderHeader " sheetId="18" r:id="rId13"/>
+    <sheet name="12. OrderDetail " sheetId="19" r:id="rId14"/>
+    <sheet name="13. FacturaHeader" sheetId="11" r:id="rId15"/>
+    <sheet name="14. FacturaDetail" sheetId="12" r:id="rId16"/>
+    <sheet name="15. FacturaPayment" sheetId="15" r:id="rId17"/>
+    <sheet name="16. CuadreHeader" sheetId="13" r:id="rId18"/>
+    <sheet name="17. CuadreDetail" sheetId="14" r:id="rId19"/>
+    <sheet name="Seguridad" sheetId="16" r:id="rId20"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="103">
   <si>
     <t>Roles</t>
   </si>
@@ -345,6 +346,12 @@
   </si>
   <si>
     <t>ErrorListId</t>
+  </si>
+  <si>
+    <t>Forma Pago</t>
+  </si>
+  <si>
+    <t>FormaPago</t>
   </si>
 </sst>
 </file>
@@ -726,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,15 +746,17 @@
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>80</v>
       </c>
@@ -773,28 +782,31 @@
         <v>20</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -840,8 +852,11 @@
       <c r="O2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -870,25 +885,28 @@
         <v>11</v>
       </c>
       <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
         <v>2</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>42</v>
       </c>
       <c r="M3" t="s">
         <v>42</v>
       </c>
       <c r="N3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" t="s">
         <v>8</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -914,28 +932,31 @@
         <v>21</v>
       </c>
       <c r="I4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>25</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>8</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>43</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>58</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>17</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -958,106 +979,109 @@
         <v>4</v>
       </c>
       <c r="J5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
         <v>26</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>34</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>44</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>59</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>40</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>27</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>35</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>26</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>4</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>23</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>36</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>23</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I8" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
         <v>28</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>37</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>45</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I9" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
         <v>4</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>38</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J10" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J11" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J12" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J13" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1070,14 +1094,15 @@
     <hyperlink ref="F1" location="'5. PermisosRoles'!A1" display="PermisosRoles"/>
     <hyperlink ref="G1" location="'6. Mesas'!A1" display="Mesas"/>
     <hyperlink ref="H1" location="'7. Monedas'!A1" display="Monedas"/>
-    <hyperlink ref="I1" location="'8. Categorias'!A1" display="Categorias"/>
-    <hyperlink ref="J1" location="'9. Productos'!A1" display="Productos"/>
-    <hyperlink ref="K1" location="'10. FacturaHeader'!A1" display="FacturaHeader"/>
-    <hyperlink ref="L1" location="'11. FacturaDetail'!A1" display="FacturaDetail"/>
-    <hyperlink ref="M1" location="'12. FacturaPayment'!A1" display="FacturaPayment"/>
-    <hyperlink ref="N1" location="'13. CuadreHeader'!A1" display="CuadreHeader"/>
-    <hyperlink ref="O1" location="'14. CuadreDetail'!A1" display="CuadreDetail"/>
+    <hyperlink ref="J1" location="'8. Categorias'!A1" display="Categorias"/>
+    <hyperlink ref="K1" location="'9. Productos'!A1" display="Productos"/>
+    <hyperlink ref="L1" location="'10. FacturaHeader'!A1" display="FacturaHeader"/>
+    <hyperlink ref="M1" location="'11. FacturaDetail'!A1" display="FacturaDetail"/>
+    <hyperlink ref="N1" location="'12. FacturaPayment'!A1" display="FacturaPayment"/>
+    <hyperlink ref="O1" location="'13. CuadreHeader'!A1" display="CuadreHeader"/>
+    <hyperlink ref="P1" location="'14. CuadreDetail'!A1" display="CuadreDetail"/>
     <hyperlink ref="A1" location="'1. ErrorList'!A1" display="ErrorList"/>
+    <hyperlink ref="I1" location="'8.5 FormaPago'!A1" display="FormaPago"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1085,6 +1110,76 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -1156,10 +1251,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
+    <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -1266,14 +1361,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -1414,7 +1509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -1532,7 +1627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -1688,7 +1783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -1806,7 +1901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -1905,7 +2000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -2028,7 +2123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -2107,143 +2202,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="2">
-        <f>SUM(D3:D9)</f>
-        <v>12552</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>33</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D9" si="0">B3*C3</f>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>450</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>10350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>62</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>496</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>74</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>84</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>26</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>78</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>1482</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:C2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2384,6 +2342,143 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="2">
+        <f>SUM(D3:D9)</f>
+        <v>12552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>33</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D9" si="0">B3*C3</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>450</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>10350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>62</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>74</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>84</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>78</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1482</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Working with product adding Referencia field
</commit_message>
<xml_diff>
--- a/PVenta.BD/PVenta.xlsx
+++ b/PVenta.BD/PVenta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" firstSheet="15" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraSist" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="104">
   <si>
     <t>Roles</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>FormaPago</t>
+  </si>
+  <si>
+    <t>Referencia</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1119,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1256,10 +1259,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,34 +1318,37 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C6">
-        <v>16.2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>57</v>
+      </c>
+      <c r="C7">
+        <v>16.2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>56</v>
@@ -1350,9 +1356,17 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed PVenta Fast Foward
</commit_message>
<xml_diff>
--- a/PVenta.BD/PVenta.xlsx
+++ b/PVenta.BD/PVenta.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="108">
   <si>
     <t>Roles</t>
   </si>
@@ -424,7 +424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,6 +434,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,21 +457,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -749,16 +757,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -781,10 +789,10 @@
       <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -837,10 +845,10 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
@@ -893,10 +901,10 @@
       <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
@@ -949,10 +957,10 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
@@ -1005,10 +1013,10 @@
       <c r="B5" t="s">
         <v>100</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="11" t="s">
         <v>101</v>
       </c>
       <c r="E5" t="s">
@@ -1058,7 +1066,7 @@
       <c r="B6" t="s">
         <v>75</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="K6" t="s">
@@ -1087,7 +1095,7 @@
       <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="K7" t="s">
@@ -1110,7 +1118,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+      <c r="D8" s="11" t="s">
         <v>8</v>
       </c>
       <c r="K8" t="s">
@@ -1128,11 +1136,14 @@
       <c r="O8" t="s">
         <v>43</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="P8" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D9" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="K9" t="s">
         <v>4</v>
       </c>
@@ -2443,9 +2454,9 @@
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2585,11 +2596,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="2">
         <f>SUM(D3:D9)</f>
         <v>12552</v>

</xml_diff>

<commit_message>
Updating Form Order Adm - adding NumOrden Property
</commit_message>
<xml_diff>
--- a/PVenta.BD/PVenta.xlsx
+++ b/PVenta.BD/PVenta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraSist" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="111">
   <si>
     <t>Roles</t>
   </si>
@@ -367,6 +367,15 @@
   </si>
   <si>
     <t>MontoEntregado</t>
+  </si>
+  <si>
+    <t>NumFactura</t>
+  </si>
+  <si>
+    <t>NumOrden</t>
+  </si>
+  <si>
+    <t>Int</t>
   </si>
 </sst>
 </file>
@@ -466,14 +475,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -755,18 +764,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -789,10 +798,10 @@
       <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -845,10 +854,10 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
@@ -901,10 +910,10 @@
       <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
@@ -957,10 +966,10 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
@@ -1013,10 +1022,10 @@
       <c r="B5" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>101</v>
       </c>
       <c r="E5" t="s">
@@ -1066,7 +1075,7 @@
       <c r="B6" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="K6" t="s">
@@ -1095,7 +1104,7 @@
       <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>13</v>
       </c>
       <c r="K7" t="s">
@@ -1118,7 +1127,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>8</v>
       </c>
       <c r="K8" t="s">
@@ -1141,7 +1150,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="9" t="s">
         <v>4</v>
       </c>
       <c r="K9" t="s">
@@ -1211,8 +1220,16 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>109</v>
+      </c>
       <c r="N14" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1258,11 +1275,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1338,11 +1355,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1408,7 +1425,7 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1418,11 +1435,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1535,7 +1552,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -1547,11 +1564,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1673,6 +1690,14 @@
       </c>
       <c r="B14" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1703,11 +1728,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1817,10 +1842,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1829,11 +1854,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1963,6 +1988,14 @@
       </c>
       <c r="B15" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1993,11 +2026,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2119,11 +2152,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2226,11 +2259,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2357,11 +2390,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2449,11 +2482,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -2596,11 +2629,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="2">
         <f>SUM(D3:D9)</f>
         <v>12552</v>
@@ -2736,11 +2769,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2816,11 +2849,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3036,11 +3069,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3117,11 +3150,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3186,11 +3219,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3258,11 +3291,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
Adding Form Ordenes and updating Form Ordenes Adm and Form Principal
</commit_message>
<xml_diff>
--- a/PVenta.BD/PVenta.xlsx
+++ b/PVenta.BD/PVenta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraSist" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,9 @@
     <sheet name="16. FacturaPayment" sheetId="15" r:id="rId17"/>
     <sheet name="17. CuadreHeader" sheetId="13" r:id="rId18"/>
     <sheet name="18. CuadreDetail" sheetId="14" r:id="rId19"/>
-    <sheet name="Seguridad" sheetId="16" r:id="rId20"/>
+    <sheet name="19. ConfigSistema" sheetId="22" r:id="rId20"/>
+    <sheet name="20, InfoDigital" sheetId="21" r:id="rId21"/>
+    <sheet name="Seguridad" sheetId="16" r:id="rId22"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="134">
   <si>
     <t>Roles</t>
   </si>
@@ -376,6 +378,75 @@
   </si>
   <si>
     <t>Int</t>
+  </si>
+  <si>
+    <t>ConfigSistema</t>
+  </si>
+  <si>
+    <t>NombreComercial</t>
+  </si>
+  <si>
+    <t>RNC</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>CalcITBIS</t>
+  </si>
+  <si>
+    <t>PorcITBIS</t>
+  </si>
+  <si>
+    <t>NumComprobanteFiscal</t>
+  </si>
+  <si>
+    <t>ComprobanteFiscal</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>InfoDigital</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>YouTube</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>MensajeOrden</t>
+  </si>
+  <si>
+    <t>MensajeFactura</t>
+  </si>
+  <si>
+    <t>ConfigInfoDigitalID</t>
+  </si>
+  <si>
+    <t>CodigoSegInactivar</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>ImprimeComandaAuto</t>
+  </si>
+  <si>
+    <t>ImprimeOrdenAuto</t>
+  </si>
+  <si>
+    <t>ImprimeFacturaAuto</t>
   </si>
 </sst>
 </file>
@@ -764,11 +835,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -789,9 +858,11 @@
     <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>76</v>
       </c>
@@ -846,8 +917,14 @@
       <c r="R1" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -902,8 +979,14 @@
       <c r="R2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -958,8 +1041,14 @@
       <c r="R3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>112</v>
+      </c>
+      <c r="T3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1014,8 +1103,14 @@
       <c r="R4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>113</v>
+      </c>
+      <c r="T4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1070,8 +1165,14 @@
       <c r="R5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>114</v>
+      </c>
+      <c r="T5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>75</v>
       </c>
@@ -1099,8 +1200,14 @@
       <c r="Q6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>125</v>
+      </c>
+      <c r="T6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -1125,8 +1232,17 @@
       <c r="P7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q7" t="s">
+        <v>4</v>
+      </c>
+      <c r="S7" t="s">
+        <v>115</v>
+      </c>
+      <c r="T7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D8" s="9" t="s">
         <v>8</v>
       </c>
@@ -1148,8 +1264,14 @@
       <c r="P8" s="6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>116</v>
+      </c>
+      <c r="T8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D9" s="9" t="s">
         <v>4</v>
       </c>
@@ -1171,8 +1293,14 @@
       <c r="P9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" t="s">
+        <v>118</v>
+      </c>
+      <c r="T9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
         <v>99</v>
       </c>
@@ -1188,8 +1316,14 @@
       <c r="O10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" t="s">
+        <v>117</v>
+      </c>
+      <c r="T10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L11" t="s">
         <v>38</v>
       </c>
@@ -1199,8 +1333,11 @@
       <c r="O11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L12" t="s">
         <v>39</v>
       </c>
@@ -1210,26 +1347,48 @@
       <c r="O12" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L13" t="s">
         <v>4</v>
       </c>
       <c r="N13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L14" t="s">
         <v>109</v>
       </c>
       <c r="N14" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N15" t="s">
         <v>108</v>
+      </c>
+      <c r="S15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S17" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1252,6 +1411,8 @@
     <hyperlink ref="L1" location="'12. OrderHeader '!A1" display="OrderHeader"/>
     <hyperlink ref="M1" location="'13. OrderDetail '!A1" display="OrderDetail"/>
     <hyperlink ref="N1" location="'14. FacturaHeader'!A1" display="FacturaHeader"/>
+    <hyperlink ref="S1" location="'19. ConfigSistema'!A1" display="ConfigSistema"/>
+    <hyperlink ref="T1" location="'20, InfoDigital'!A1" display="InfoDigital"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1425,7 +1586,7 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -2381,7 +2542,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2617,6 +2778,341 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EstructuraSist!A1" display="CuadreDetail"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EstructuraSist!A1" display="CuadreDetail"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Adding ConfigSistema, InfoDigital and TypeInfo Models / updating xls / Adding new models to DB Context
</commit_message>
<xml_diff>
--- a/PVenta.BD/PVenta.xlsx
+++ b/PVenta.BD/PVenta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" firstSheet="18" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraSist" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,10 @@
     <sheet name="16. FacturaPayment" sheetId="15" r:id="rId17"/>
     <sheet name="17. CuadreHeader" sheetId="13" r:id="rId18"/>
     <sheet name="18. CuadreDetail" sheetId="14" r:id="rId19"/>
-    <sheet name="19. ConfigSistema" sheetId="22" r:id="rId20"/>
-    <sheet name="20, InfoDigital" sheetId="21" r:id="rId21"/>
-    <sheet name="Seguridad" sheetId="16" r:id="rId22"/>
+    <sheet name="19. TypeInfo" sheetId="21" r:id="rId20"/>
+    <sheet name="20. InfoDigital" sheetId="23" r:id="rId21"/>
+    <sheet name="21. ConfigSistema" sheetId="22" r:id="rId22"/>
+    <sheet name="Seguridad" sheetId="16" r:id="rId23"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="139">
   <si>
     <t>Roles</t>
   </si>
@@ -447,6 +448,21 @@
   </si>
   <si>
     <t>ImprimeFacturaAuto</t>
+  </si>
+  <si>
+    <t>TypeInfo</t>
+  </si>
+  <si>
+    <t>FaceBook</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>RelacionID</t>
+  </si>
+  <si>
+    <t>TypeInfoID</t>
   </si>
 </sst>
 </file>
@@ -835,9 +851,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1042,7 +1060,7 @@
         <v>46</v>
       </c>
       <c r="S3" t="s">
-        <v>112</v>
+        <v>2</v>
       </c>
       <c r="T3" t="s">
         <v>128</v>
@@ -1104,7 +1122,7 @@
         <v>42</v>
       </c>
       <c r="S4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T4" t="s">
         <v>11</v>
@@ -1166,7 +1184,7 @@
         <v>19</v>
       </c>
       <c r="S5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T5" t="s">
         <v>119</v>
@@ -1201,7 +1219,7 @@
         <v>44</v>
       </c>
       <c r="S6" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="T6" t="s">
         <v>120</v>
@@ -1236,7 +1254,7 @@
         <v>4</v>
       </c>
       <c r="S7" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="T7" t="s">
         <v>122</v>
@@ -1265,7 +1283,7 @@
         <v>107</v>
       </c>
       <c r="S8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T8" t="s">
         <v>123</v>
@@ -1294,7 +1312,7 @@
         <v>4</v>
       </c>
       <c r="S9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T9" t="s">
         <v>124</v>
@@ -1317,7 +1335,7 @@
         <v>39</v>
       </c>
       <c r="S10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="T10" t="s">
         <v>4</v>
@@ -1334,7 +1352,7 @@
         <v>4</v>
       </c>
       <c r="S11" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1348,7 +1366,7 @@
         <v>105</v>
       </c>
       <c r="S12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1359,7 +1377,7 @@
         <v>4</v>
       </c>
       <c r="S13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1370,7 +1388,7 @@
         <v>95</v>
       </c>
       <c r="S14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1378,16 +1396,21 @@
         <v>108</v>
       </c>
       <c r="S15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="S16" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S18" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2781,25 +2804,25 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -2810,159 +2833,55 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>48</v>
       </c>
       <c r="C4">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9">
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>133</v>
-      </c>
-      <c r="B16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>54</v>
+      <c r="E5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2981,10 +2900,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3020,7 +2939,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
@@ -3028,10 +2947,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>50</v>
@@ -3039,7 +2958,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
@@ -3050,53 +2969,9 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3112,6 +2987,225 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EstructuraSist!A1" display="CuadreDetail"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Adding new property 'permiteAdicional' to Producto Model, to permit define additional productos to the order
</commit_message>
<xml_diff>
--- a/PVenta.BD/PVenta.xlsx
+++ b/PVenta.BD/PVenta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" firstSheet="18" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraSist" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="140">
   <si>
     <t>Roles</t>
   </si>
@@ -463,6 +463,9 @@
   </si>
   <si>
     <t>TypeInfoID</t>
+  </si>
+  <si>
+    <t>permiteAdicional</t>
   </si>
 </sst>
 </file>
@@ -853,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,6 +1345,9 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>139</v>
+      </c>
       <c r="L11" t="s">
         <v>38</v>
       </c>
@@ -1607,7 +1613,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -1717,6 +1723,14 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2993,7 +3007,7 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update PVenta structure and Postman Collection
</commit_message>
<xml_diff>
--- a/PVenta.BD/PVenta.xlsx
+++ b/PVenta.BD/PVenta.xlsx
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,16 +866,16 @@
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" style="9" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -896,37 +896,37 @@
       <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="8" t="s">
         <v>30</v>
       </c>
       <c r="P1" s="5" t="s">
@@ -958,37 +958,37 @@
       <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="E2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="P2" t="s">
@@ -1020,37 +1020,37 @@
       <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="9" t="s">
         <v>40</v>
       </c>
       <c r="P3" t="s">
@@ -1082,37 +1082,37 @@
       <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="9" t="s">
         <v>41</v>
       </c>
       <c r="P4" t="s">
@@ -1144,37 +1144,37 @@
       <c r="D5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="9" t="s">
         <v>42</v>
       </c>
       <c r="P5" t="s">
@@ -1200,19 +1200,19 @@
       <c r="D6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P6" t="s">
@@ -1235,19 +1235,19 @@
       <c r="D7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="9" t="s">
         <v>21</v>
       </c>
       <c r="P7" t="s">
@@ -1267,19 +1267,19 @@
       <c r="D8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="9" t="s">
         <v>43</v>
       </c>
       <c r="P8" s="6" t="s">
@@ -1296,19 +1296,19 @@
       <c r="D9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="9" t="s">
         <v>4</v>
       </c>
       <c r="P9" t="s">
@@ -1322,19 +1322,19 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K10" t="s">
+      <c r="K10" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="9" t="s">
         <v>39</v>
       </c>
       <c r="S10" t="s">
@@ -1345,16 +1345,16 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K11" t="s">
+      <c r="K11" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" s="9" t="s">
         <v>4</v>
       </c>
       <c r="S11" t="s">
@@ -1362,13 +1362,13 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L12" t="s">
+      <c r="L12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="9" t="s">
         <v>105</v>
       </c>
       <c r="S12" t="s">
@@ -1376,10 +1376,10 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L13" t="s">
+      <c r="L13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="9" t="s">
         <v>4</v>
       </c>
       <c r="S13" t="s">
@@ -1387,10 +1387,10 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L14" t="s">
+      <c r="L14" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="9" t="s">
         <v>95</v>
       </c>
       <c r="S14" t="s">
@@ -1398,7 +1398,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N15" t="s">
+      <c r="N15" s="9" t="s">
         <v>108</v>
       </c>
       <c r="S15" t="s">

</xml_diff>

<commit_message>
Adding new property to FormaPago (AceptaCambio)
</commit_message>
<xml_diff>
--- a/PVenta.BD/PVenta.xlsx
+++ b/PVenta.BD/PVenta.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="141">
   <si>
     <t>Roles</t>
   </si>
@@ -246,9 +246,6 @@
     <t>FacturaHID</t>
   </si>
   <si>
-    <t>FacturaDID</t>
-  </si>
-  <si>
     <t>MontoPago</t>
   </si>
   <si>
@@ -466,6 +463,12 @@
   </si>
   <si>
     <t>permiteAdicional</t>
+  </si>
+  <si>
+    <t>FormaPagoID</t>
+  </si>
+  <si>
+    <t>AceptaCambio</t>
   </si>
 </sst>
 </file>
@@ -856,9 +859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -885,7 +886,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>15</v>
@@ -909,7 +910,7 @@
         <v>18</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>20</v>
@@ -918,10 +919,10 @@
         <v>22</v>
       </c>
       <c r="L1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>28</v>
@@ -939,10 +940,10 @@
         <v>31</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1009,7 +1010,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1021,7 +1022,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>13</v>
@@ -1045,7 +1046,7 @@
         <v>16</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>16</v>
@@ -1066,12 +1067,12 @@
         <v>2</v>
       </c>
       <c r="T3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1089,13 +1090,13 @@
         <v>14</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>21</v>
@@ -1116,7 +1117,7 @@
         <v>41</v>
       </c>
       <c r="P4" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="Q4" t="s">
         <v>16</v>
@@ -1125,7 +1126,7 @@
         <v>42</v>
       </c>
       <c r="S4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T4" t="s">
         <v>11</v>
@@ -1136,13 +1137,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>4</v>
@@ -1178,7 +1179,7 @@
         <v>42</v>
       </c>
       <c r="P5" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="Q5" t="s">
         <v>38</v>
@@ -1187,19 +1188,22 @@
         <v>19</v>
       </c>
       <c r="S5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="I6" s="9" t="s">
+        <v>140</v>
+      </c>
       <c r="K6" s="9" t="s">
         <v>25</v>
       </c>
@@ -1215,17 +1219,17 @@
       <c r="O6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="P6" t="s">
-        <v>72</v>
+      <c r="P6" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="Q6" t="s">
         <v>44</v>
       </c>
       <c r="S6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1251,16 +1255,16 @@
         <v>21</v>
       </c>
       <c r="P7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q7" t="s">
         <v>4</v>
       </c>
       <c r="S7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1283,13 +1287,13 @@
         <v>43</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -1315,15 +1319,15 @@
         <v>4</v>
       </c>
       <c r="S9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="K10" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>37</v>
@@ -1338,7 +1342,7 @@
         <v>39</v>
       </c>
       <c r="S10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T10" t="s">
         <v>4</v>
@@ -1346,7 +1350,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="K11" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>38</v>
@@ -1358,7 +1362,7 @@
         <v>4</v>
       </c>
       <c r="S11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1369,10 +1373,10 @@
         <v>39</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1383,36 +1387,36 @@
         <v>4</v>
       </c>
       <c r="S13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L14" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N15" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="S16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="19:19" x14ac:dyDescent="0.25">
@@ -1453,7 +1457,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -1461,12 +1465,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1503,7 +1507,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>48</v>
@@ -1514,6 +1518,14 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1674,7 +1686,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
@@ -1728,7 +1740,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B12" t="s">
         <v>54</v>
@@ -1763,7 +1775,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1892,10 +1904,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
         <v>109</v>
-      </c>
-      <c r="B15" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1927,7 +1939,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1953,7 +1965,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
@@ -2079,7 +2091,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
@@ -2190,10 +2202,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2338,7 +2350,7 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -2385,47 +2397,39 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="C7">
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2504,10 +2508,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C6" s="3">
         <v>16.2</v>
@@ -2542,7 +2546,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
@@ -2623,7 +2627,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>47</v>
@@ -2681,7 +2685,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2700,10 +2704,10 @@
         <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2714,38 +2718,38 @@
         <v>47</v>
       </c>
       <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
         <v>77</v>
-      </c>
-      <c r="F3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
         <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2756,50 +2760,50 @@
         <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" t="s">
         <v>89</v>
-      </c>
-      <c r="F9" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" t="s">
         <v>80</v>
-      </c>
-      <c r="F10" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" t="s">
         <v>82</v>
-      </c>
-      <c r="F11" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2831,7 +2835,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2855,7 +2859,7 @@
         <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2869,7 +2873,7 @@
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2880,22 +2884,22 @@
         <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2927,7 +2931,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2953,7 +2957,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
@@ -2961,7 +2965,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
         <v>47</v>
@@ -3018,7 +3022,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -3055,7 +3059,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
         <v>48</v>
@@ -3066,7 +3070,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
@@ -3077,7 +3081,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
@@ -3088,7 +3092,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
@@ -3099,7 +3103,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
         <v>47</v>
@@ -3107,7 +3111,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
         <v>54</v>
@@ -3115,7 +3119,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
         <v>55</v>
@@ -3126,7 +3130,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
         <v>48</v>
@@ -3137,15 +3141,15 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
         <v>48</v>
@@ -3156,7 +3160,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B15" t="s">
         <v>48</v>
@@ -3167,7 +3171,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
         <v>54</v>
@@ -3175,7 +3179,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
         <v>54</v>
@@ -3183,7 +3187,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
         <v>54</v>
@@ -3191,7 +3195,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
@@ -3525,7 +3529,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
@@ -3634,7 +3638,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
@@ -3642,7 +3646,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
         <v>53</v>
@@ -3700,7 +3704,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>48</v>

</xml_diff>